<commit_message>
there's a issue with next_link().
</commit_message>
<xml_diff>
--- a/seo.xlsx
+++ b/seo.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,7 +462,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>https://m.muenchenmusik.de</t>
+          <t>https://www.headstruggle.de</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -472,36 +472,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t xml:space="preserve">
-        Konzerte in München - Tickets bei MünchenMusik
-</t>
+          <t>The Struggles in my Head</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>https://m.muenchenmusik.de</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>Konzertkarten für klassische Musik in München - Tickets online bestellen - Konzerte und Theater im Prinzregententheater, der Residenz und der Philharmonie.</t>
-        </is>
-      </c>
-      <c r="E3" t="n">
-        <v>155</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>